<commit_message>
Revise leg number to cm
</commit_message>
<xml_diff>
--- a/index.md/GeoAngles.md/res/measurements.xlsx
+++ b/index.md/GeoAngles.md/res/measurements.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sephi\Desktop\CreateJS Projects\GeoAngles.md\res\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sephi\Desktop\GitHub Manipulatives\mpcender.github.io\index.md\GeoAngles.md\res\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60FF6FA9-7D73-46CE-916E-CA1D7CC2BA7B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CC79E20-F49D-4F19-827E-40F9ED243FE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-14310" yWindow="-3750" windowWidth="11565" windowHeight="13440" xr2:uid="{442C4845-08EA-4FFF-9735-239B91B9B18C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{442C4845-08EA-4FFF-9735-239B91B9B18C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -424,10 +424,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77ED9FCF-ADAD-4725-A8B2-A7F3204100A2}">
-  <dimension ref="A1:F12"/>
+  <dimension ref="A1:J21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -435,7 +435,7 @@
     <col min="2" max="2" width="10.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>6</v>
       </c>
@@ -449,7 +449,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -467,8 +467,15 @@
         <f>ROUND(E2,0)</f>
         <v>902</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H2">
+        <v>1800</v>
+      </c>
+      <c r="I2">
+        <f>H2/2</f>
+        <v>900</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -487,8 +494,19 @@
         <f t="shared" ref="F3:F7" si="0">ROUND(E3,0)</f>
         <v>781</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H3">
+        <v>1558</v>
+      </c>
+      <c r="I3">
+        <f t="shared" ref="I3:I7" si="1">H3/2</f>
+        <v>779</v>
+      </c>
+      <c r="J3">
+        <f>I3/I2</f>
+        <v>0.86555555555555552</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -496,19 +514,30 @@
         <v>10</v>
       </c>
       <c r="C4">
-        <f t="shared" ref="C4:C6" si="1">B4/B3</f>
+        <f t="shared" ref="C4:C6" si="2">B4/B3</f>
         <v>0.81699346405228757</v>
       </c>
       <c r="E4">
-        <f t="shared" ref="E4:E7" si="2">E3*C4</f>
+        <f t="shared" ref="E4:E7" si="3">E3*C4</f>
         <v>637.90664780763791</v>
       </c>
       <c r="F4">
         <f t="shared" si="0"/>
         <v>638</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H4">
+        <v>1272</v>
+      </c>
+      <c r="I4">
+        <f t="shared" si="1"/>
+        <v>636</v>
+      </c>
+      <c r="J4">
+        <f t="shared" ref="J4:J7" si="4">I4/I3</f>
+        <v>0.81643132220795889</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -516,19 +545,30 @@
         <v>8.66</v>
       </c>
       <c r="C5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.86599999999999999</v>
       </c>
       <c r="E5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>552.42715700141446</v>
       </c>
       <c r="F5">
         <f t="shared" si="0"/>
         <v>552</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H5">
+        <v>1100</v>
+      </c>
+      <c r="I5">
+        <f t="shared" si="1"/>
+        <v>550</v>
+      </c>
+      <c r="J5">
+        <f t="shared" si="4"/>
+        <v>0.86477987421383651</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -536,19 +576,30 @@
         <v>7.07</v>
       </c>
       <c r="C6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.81639722863741337</v>
       </c>
       <c r="E6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>451</v>
       </c>
       <c r="F6">
         <f t="shared" si="0"/>
         <v>451</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H6">
+        <v>898</v>
+      </c>
+      <c r="I6">
+        <f t="shared" si="1"/>
+        <v>449</v>
+      </c>
+      <c r="J6">
+        <f t="shared" si="4"/>
+        <v>0.8163636363636364</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -560,15 +611,42 @@
         <v>0.70721357850070721</v>
       </c>
       <c r="E7">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>318.95332390381895</v>
       </c>
       <c r="F7">
         <f t="shared" si="0"/>
         <v>319</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H7">
+        <v>634</v>
+      </c>
+      <c r="I7">
+        <f t="shared" si="1"/>
+        <v>317</v>
+      </c>
+      <c r="J7">
+        <f t="shared" si="4"/>
+        <v>0.70601336302895323</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F9">
+        <v>378.4</v>
+      </c>
+      <c r="G9">
+        <f>FLOOR(F9/10.5,2)</f>
+        <v>36</v>
+      </c>
+      <c r="I9">
+        <v>900</v>
+      </c>
+      <c r="J9">
+        <f>I9/25</f>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>10</v>
       </c>
@@ -579,8 +657,22 @@
         <f>B10*0.4</f>
         <v>9.2000000000000011</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F10">
+        <v>330</v>
+      </c>
+      <c r="G10">
+        <f t="shared" ref="G10:G13" si="5">FLOOR(F10/10.5,2)</f>
+        <v>30</v>
+      </c>
+      <c r="I10">
+        <v>775</v>
+      </c>
+      <c r="J10">
+        <f t="shared" ref="J10:J14" si="6">I10/25</f>
+        <v>31</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>11</v>
       </c>
@@ -588,11 +680,25 @@
         <v>27</v>
       </c>
       <c r="C11">
-        <f t="shared" ref="C11:C12" si="3">B11*0.4</f>
+        <f t="shared" ref="C11:C12" si="7">B11*0.4</f>
         <v>10.8</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F11">
+        <v>272.8</v>
+      </c>
+      <c r="G11">
+        <f t="shared" si="5"/>
+        <v>24</v>
+      </c>
+      <c r="I11">
+        <v>625</v>
+      </c>
+      <c r="J11">
+        <f t="shared" si="6"/>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>12</v>
       </c>
@@ -600,8 +706,164 @@
         <v>23</v>
       </c>
       <c r="C12">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>9.2000000000000011</v>
+      </c>
+      <c r="F12">
+        <v>238.4</v>
+      </c>
+      <c r="G12">
+        <f t="shared" si="5"/>
+        <v>22</v>
+      </c>
+      <c r="I12">
+        <v>550</v>
+      </c>
+      <c r="J12">
+        <f t="shared" si="6"/>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F13">
+        <v>198</v>
+      </c>
+      <c r="G13">
+        <f t="shared" si="5"/>
+        <v>18</v>
+      </c>
+      <c r="I13">
+        <v>450</v>
+      </c>
+      <c r="J13">
+        <f t="shared" si="6"/>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F14">
+        <v>145.19999999999999</v>
+      </c>
+      <c r="G14">
+        <f>FLOOR(F14/10.5,2)</f>
+        <v>12</v>
+      </c>
+      <c r="I14">
+        <v>325</v>
+      </c>
+      <c r="J14">
+        <f t="shared" si="6"/>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B16">
+        <v>14.14</v>
+      </c>
+      <c r="F16">
+        <v>378.4</v>
+      </c>
+      <c r="G16">
+        <v>34.57</v>
+      </c>
+      <c r="H16">
+        <f>F16/G16</f>
+        <v>10.945906855655192</v>
+      </c>
+    </row>
+    <row r="17" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B17">
+        <v>12.24</v>
+      </c>
+      <c r="F17">
+        <v>330</v>
+      </c>
+      <c r="G17">
+        <v>34.57</v>
+      </c>
+      <c r="H17">
+        <f t="shared" ref="H17:H21" si="8">F17/G17</f>
+        <v>9.5458490020248767</v>
+      </c>
+      <c r="J17">
+        <f>F17/4.2</f>
+        <v>78.571428571428569</v>
+      </c>
+    </row>
+    <row r="18" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B18">
+        <v>10</v>
+      </c>
+      <c r="F18">
+        <v>272.8</v>
+      </c>
+      <c r="G18">
+        <v>34.57</v>
+      </c>
+      <c r="H18">
+        <f t="shared" si="8"/>
+        <v>7.8912351750072318</v>
+      </c>
+      <c r="J18">
+        <f t="shared" ref="J18:J21" si="9">F18/4.2</f>
+        <v>64.952380952380949</v>
+      </c>
+    </row>
+    <row r="19" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B19">
+        <v>8.66</v>
+      </c>
+      <c r="F19">
+        <v>238.4</v>
+      </c>
+      <c r="G19">
+        <v>34.57</v>
+      </c>
+      <c r="H19">
+        <f t="shared" si="8"/>
+        <v>6.8961527335840325</v>
+      </c>
+      <c r="J19">
+        <f t="shared" si="9"/>
+        <v>56.761904761904759</v>
+      </c>
+    </row>
+    <row r="20" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B20">
+        <v>7.07</v>
+      </c>
+      <c r="F20">
+        <v>198</v>
+      </c>
+      <c r="G20">
+        <v>34.57</v>
+      </c>
+      <c r="H20">
+        <f t="shared" si="8"/>
+        <v>5.7275094012149266</v>
+      </c>
+      <c r="J20">
+        <f t="shared" si="9"/>
+        <v>47.142857142857139</v>
+      </c>
+    </row>
+    <row r="21" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B21">
+        <v>5</v>
+      </c>
+      <c r="F21">
+        <v>145.19999999999999</v>
+      </c>
+      <c r="G21">
+        <v>34.57</v>
+      </c>
+      <c r="H21">
+        <f t="shared" si="8"/>
+        <v>4.2001735608909456</v>
+      </c>
+      <c r="J21">
+        <f t="shared" si="9"/>
+        <v>34.571428571428569</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Leg length and text display update
</commit_message>
<xml_diff>
--- a/index.md/GeoAngles.md/res/measurements.xlsx
+++ b/index.md/GeoAngles.md/res/measurements.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sephi\Desktop\GitHub Manipulatives\mpcender.github.io\index.md\GeoAngles.md\res\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CC79E20-F49D-4F19-827E-40F9ED243FE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71774CEF-E4A1-4A20-A3D2-F71CEDBE9585}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{442C4845-08EA-4FFF-9735-239B91B9B18C}"/>
+    <workbookView xWindow="5430" yWindow="2595" windowWidth="6810" windowHeight="11385" xr2:uid="{442C4845-08EA-4FFF-9735-239B91B9B18C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>red</t>
   </si>
@@ -73,14 +73,37 @@
   </si>
   <si>
     <t>y</t>
+  </si>
+  <si>
+    <t>width</t>
+  </si>
+  <si>
+    <t>center circ</t>
+  </si>
+  <si>
+    <t>circ diam</t>
+  </si>
+  <si>
+    <t>circ to edge</t>
+  </si>
+  <si>
+    <t xml:space="preserve">curve </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -108,8 +131,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -424,10 +448,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77ED9FCF-ADAD-4725-A8B2-A7F3204100A2}">
-  <dimension ref="A1:J21"/>
+  <dimension ref="A1:G27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+    <sheetView tabSelected="1" topLeftCell="B4" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -435,7 +459,7 @@
     <col min="2" max="2" width="10.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>6</v>
       </c>
@@ -449,7 +473,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -457,25 +481,21 @@
         <v>14.14</v>
       </c>
       <c r="D2">
-        <v>946</v>
+        <v>26.76</v>
       </c>
       <c r="E2">
-        <f>D2-44</f>
-        <v>902</v>
+        <v>378.4</v>
       </c>
       <c r="F2">
-        <f>ROUND(E2,0)</f>
-        <v>902</v>
-      </c>
-      <c r="H2">
-        <v>1800</v>
-      </c>
-      <c r="I2">
-        <f>H2/2</f>
-        <v>900</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+        <f>ROUND(E2/D$2,2)</f>
+        <v>14.14</v>
+      </c>
+      <c r="G2">
+        <f>E2-(9.2*2)</f>
+        <v>360</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -487,26 +507,18 @@
         <v>0.86562942008486565</v>
       </c>
       <c r="E3">
-        <f>E2*C3</f>
-        <v>780.79773691654884</v>
+        <v>327.60000000000002</v>
       </c>
       <c r="F3">
-        <f t="shared" ref="F3:F7" si="0">ROUND(E3,0)</f>
-        <v>781</v>
-      </c>
-      <c r="H3">
-        <v>1558</v>
-      </c>
-      <c r="I3">
-        <f t="shared" ref="I3:I7" si="1">H3/2</f>
-        <v>779</v>
-      </c>
-      <c r="J3">
-        <f>I3/I2</f>
-        <v>0.86555555555555552</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+        <f t="shared" ref="F3:F7" si="0">ROUND(E3/D$2,2)</f>
+        <v>12.24</v>
+      </c>
+      <c r="G3">
+        <f t="shared" ref="G3:G7" si="1">E3-(9.2*2)</f>
+        <v>309.20000000000005</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -518,26 +530,18 @@
         <v>0.81699346405228757</v>
       </c>
       <c r="E4">
-        <f t="shared" ref="E4:E7" si="3">E3*C4</f>
-        <v>637.90664780763791</v>
+        <v>267.60000000000002</v>
       </c>
       <c r="F4">
         <f t="shared" si="0"/>
-        <v>638</v>
-      </c>
-      <c r="H4">
-        <v>1272</v>
-      </c>
-      <c r="I4">
+        <v>10</v>
+      </c>
+      <c r="G4">
         <f t="shared" si="1"/>
-        <v>636</v>
-      </c>
-      <c r="J4">
-        <f t="shared" ref="J4:J7" si="4">I4/I3</f>
-        <v>0.81643132220795889</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+        <v>249.20000000000002</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -549,26 +553,18 @@
         <v>0.86599999999999999</v>
       </c>
       <c r="E5">
-        <f t="shared" si="3"/>
-        <v>552.42715700141446</v>
+        <v>231.6</v>
       </c>
       <c r="F5">
         <f t="shared" si="0"/>
-        <v>552</v>
-      </c>
-      <c r="H5">
-        <v>1100</v>
-      </c>
-      <c r="I5">
+        <v>8.65</v>
+      </c>
+      <c r="G5">
         <f t="shared" si="1"/>
-        <v>550</v>
-      </c>
-      <c r="J5">
-        <f t="shared" si="4"/>
-        <v>0.86477987421383651</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+        <v>213.2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -580,26 +576,18 @@
         <v>0.81639722863741337</v>
       </c>
       <c r="E6">
-        <f t="shared" si="3"/>
-        <v>451</v>
+        <v>189.2</v>
       </c>
       <c r="F6">
         <f t="shared" si="0"/>
-        <v>451</v>
-      </c>
-      <c r="H6">
-        <v>898</v>
-      </c>
-      <c r="I6">
+        <v>7.07</v>
+      </c>
+      <c r="G6">
         <f t="shared" si="1"/>
-        <v>449</v>
-      </c>
-      <c r="J6">
-        <f t="shared" si="4"/>
-        <v>0.8163636363636364</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+        <v>170.79999999999998</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -611,42 +599,18 @@
         <v>0.70721357850070721</v>
       </c>
       <c r="E7">
-        <f t="shared" si="3"/>
-        <v>318.95332390381895</v>
+        <v>134</v>
       </c>
       <c r="F7">
         <f t="shared" si="0"/>
-        <v>319</v>
-      </c>
-      <c r="H7">
-        <v>634</v>
-      </c>
-      <c r="I7">
+        <v>5.01</v>
+      </c>
+      <c r="G7">
         <f t="shared" si="1"/>
-        <v>317</v>
-      </c>
-      <c r="J7">
-        <f t="shared" si="4"/>
-        <v>0.70601336302895323</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="F9">
-        <v>378.4</v>
-      </c>
-      <c r="G9">
-        <f>FLOOR(F9/10.5,2)</f>
-        <v>36</v>
-      </c>
-      <c r="I9">
-        <v>900</v>
-      </c>
-      <c r="J9">
-        <f>I9/25</f>
-        <v>36</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+        <v>115.6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>10</v>
       </c>
@@ -657,22 +621,19 @@
         <f>B10*0.4</f>
         <v>9.2000000000000011</v>
       </c>
+      <c r="E10">
+        <v>396.8</v>
+      </c>
       <c r="F10">
-        <v>330</v>
+        <f t="shared" ref="F10:F14" si="3">ROUND((E10-153)/47,0)</f>
+        <v>5</v>
       </c>
       <c r="G10">
-        <f t="shared" ref="G10:G13" si="5">FLOOR(F10/10.5,2)</f>
-        <v>30</v>
-      </c>
-      <c r="I10">
-        <v>775</v>
-      </c>
-      <c r="J10">
-        <f t="shared" ref="J10:J14" si="6">I10/25</f>
-        <v>31</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+        <f t="shared" ref="G10:G14" si="4">(E10-152)/48</f>
+        <v>5.1000000000000005</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>11</v>
       </c>
@@ -680,25 +641,22 @@
         <v>27</v>
       </c>
       <c r="C11">
-        <f t="shared" ref="C11:C12" si="7">B11*0.4</f>
+        <f t="shared" ref="C11:C12" si="5">B11*0.4</f>
         <v>10.8</v>
       </c>
+      <c r="E11">
+        <v>346</v>
+      </c>
       <c r="F11">
-        <v>272.8</v>
+        <f t="shared" si="3"/>
+        <v>4</v>
       </c>
       <c r="G11">
-        <f t="shared" si="5"/>
-        <v>24</v>
-      </c>
-      <c r="I11">
-        <v>625</v>
-      </c>
-      <c r="J11">
-        <f t="shared" si="6"/>
-        <v>25</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>4.041666666666667</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>12</v>
       </c>
@@ -706,167 +664,184 @@
         <v>23</v>
       </c>
       <c r="C12">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>9.2000000000000011</v>
       </c>
+      <c r="E12">
+        <v>286</v>
+      </c>
       <c r="F12">
-        <v>238.4</v>
+        <f t="shared" si="3"/>
+        <v>3</v>
       </c>
       <c r="G12">
-        <f t="shared" si="5"/>
-        <v>22</v>
-      </c>
-      <c r="I12">
-        <v>550</v>
-      </c>
-      <c r="J12">
-        <f t="shared" si="6"/>
-        <v>22</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>2.7916666666666665</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E13">
+        <v>250</v>
+      </c>
       <c r="F13">
-        <v>198</v>
+        <f t="shared" si="3"/>
+        <v>2</v>
       </c>
       <c r="G13">
-        <f t="shared" si="5"/>
-        <v>18</v>
-      </c>
-      <c r="I13">
-        <v>450</v>
-      </c>
-      <c r="J13">
-        <f t="shared" si="6"/>
-        <v>18</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>2.0416666666666665</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E14">
+        <v>207.6</v>
+      </c>
       <c r="F14">
-        <v>145.19999999999999</v>
+        <f t="shared" si="3"/>
+        <v>1</v>
       </c>
       <c r="G14">
-        <f>FLOOR(F14/10.5,2)</f>
-        <v>12</v>
-      </c>
-      <c r="I14">
-        <v>325</v>
-      </c>
-      <c r="J14">
-        <f t="shared" si="6"/>
-        <v>13</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>1.1583333333333332</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C15">
+        <f>946/B16</f>
+        <v>66.902404526166904</v>
+      </c>
+      <c r="E15">
+        <v>152.4</v>
+      </c>
+      <c r="F15">
+        <f>ROUND((E15-153)/47,0)</f>
+        <v>0</v>
+      </c>
+      <c r="G15">
+        <f>(E15-152)/48</f>
+        <v>8.3333333333334512E-3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B16">
         <v>14.14</v>
       </c>
-      <c r="F16">
-        <v>378.4</v>
-      </c>
-      <c r="G16">
-        <v>34.57</v>
-      </c>
-      <c r="H16">
-        <f>F16/G16</f>
-        <v>10.945906855655192</v>
-      </c>
-    </row>
-    <row r="17" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="C16">
+        <f>B16*C$15</f>
+        <v>946.00000000000011</v>
+      </c>
+      <c r="D16">
+        <f>ROUND(C16,0)+46</f>
+        <v>992</v>
+      </c>
+    </row>
+    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B17">
         <v>12.24</v>
       </c>
-      <c r="F17">
-        <v>330</v>
-      </c>
-      <c r="G17">
-        <v>34.57</v>
-      </c>
-      <c r="H17">
-        <f t="shared" ref="H17:H21" si="8">F17/G17</f>
-        <v>9.5458490020248767</v>
-      </c>
-      <c r="J17">
-        <f>F17/4.2</f>
-        <v>78.571428571428569</v>
-      </c>
-    </row>
-    <row r="18" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="C17">
+        <f t="shared" ref="C17:C21" si="6">B17*C$15</f>
+        <v>818.88543140028287</v>
+      </c>
+      <c r="D17">
+        <f t="shared" ref="D17:D21" si="7">ROUND(C17,0)+46</f>
+        <v>865</v>
+      </c>
+    </row>
+    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B18">
         <v>10</v>
       </c>
-      <c r="F18">
-        <v>272.8</v>
-      </c>
-      <c r="G18">
-        <v>34.57</v>
-      </c>
-      <c r="H18">
-        <f t="shared" si="8"/>
-        <v>7.8912351750072318</v>
-      </c>
-      <c r="J18">
-        <f t="shared" ref="J18:J21" si="9">F18/4.2</f>
-        <v>64.952380952380949</v>
-      </c>
-    </row>
-    <row r="19" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="C18">
+        <f t="shared" si="6"/>
+        <v>669.02404526166902</v>
+      </c>
+      <c r="D18">
+        <f t="shared" si="7"/>
+        <v>715</v>
+      </c>
+    </row>
+    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B19">
         <v>8.66</v>
       </c>
-      <c r="F19">
-        <v>238.4</v>
-      </c>
-      <c r="G19">
-        <v>34.57</v>
-      </c>
-      <c r="H19">
-        <f t="shared" si="8"/>
-        <v>6.8961527335840325</v>
-      </c>
-      <c r="J19">
-        <f t="shared" si="9"/>
-        <v>56.761904761904759</v>
-      </c>
-    </row>
-    <row r="20" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="C19">
+        <f t="shared" si="6"/>
+        <v>579.37482319660535</v>
+      </c>
+      <c r="D19">
+        <f t="shared" si="7"/>
+        <v>625</v>
+      </c>
+    </row>
+    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B20">
         <v>7.07</v>
       </c>
-      <c r="F20">
-        <v>198</v>
-      </c>
-      <c r="G20">
-        <v>34.57</v>
-      </c>
-      <c r="H20">
-        <f t="shared" si="8"/>
-        <v>5.7275094012149266</v>
-      </c>
-      <c r="J20">
-        <f t="shared" si="9"/>
-        <v>47.142857142857139</v>
-      </c>
-    </row>
-    <row r="21" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="C20">
+        <f t="shared" si="6"/>
+        <v>473.00000000000006</v>
+      </c>
+      <c r="D20">
+        <f t="shared" si="7"/>
+        <v>519</v>
+      </c>
+    </row>
+    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B21">
         <v>5</v>
       </c>
-      <c r="F21">
-        <v>145.19999999999999</v>
-      </c>
-      <c r="G21">
-        <v>34.57</v>
-      </c>
-      <c r="H21">
-        <f t="shared" si="8"/>
-        <v>4.2001735608909456</v>
-      </c>
-      <c r="J21">
-        <f t="shared" si="9"/>
-        <v>34.571428571428569</v>
+      <c r="C21">
+        <f t="shared" si="6"/>
+        <v>334.51202263083451</v>
+      </c>
+      <c r="D21">
+        <f t="shared" si="7"/>
+        <v>381</v>
+      </c>
+    </row>
+    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B23" t="s">
+        <v>13</v>
+      </c>
+      <c r="C23" s="1">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B24" t="s">
+        <v>14</v>
+      </c>
+      <c r="C24">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="25" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B25" t="s">
+        <v>15</v>
+      </c>
+      <c r="C25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B26" t="s">
+        <v>16</v>
+      </c>
+      <c r="C26">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="27" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B27" t="s">
+        <v>17</v>
+      </c>
+      <c r="C27">
+        <v>19</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>